<commit_message>
agregados comentarios del tester
</commit_message>
<xml_diff>
--- a/Test Documentation/Sprint 3 Test Doc TM52.xlsx
+++ b/Test Documentation/Sprint 3 Test Doc TM52.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Test User-Story ID</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>ID: tomasporcaro22@gmail.com password: 123</t>
+  </si>
+  <si>
+    <t>Verifico que se crea de forma aletoria el token y es traido desde el back</t>
   </si>
 </sst>
 </file>
@@ -569,154 +572,154 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -940,7 +943,7 @@
   <dimension ref="A1:N153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -951,17 +954,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="72"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="25" t="s">
         <v>24</v>
       </c>
@@ -974,21 +977,21 @@
       <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="72"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="86" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -1004,44 +1007,46 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="78">
+      <c r="B6" s="36"/>
+      <c r="C6" s="33">
         <v>44161</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
@@ -1060,157 +1065,157 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="80" t="s">
+      <c r="G8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
     </row>
     <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>56</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="79"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="2"/>
       <c r="F9" s="9">
         <v>56</v>
       </c>
-      <c r="G9" s="81" t="s">
+      <c r="G9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="79"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>64</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="70"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="2"/>
       <c r="F10" s="11">
         <v>64</v>
       </c>
-      <c r="G10" s="81" t="s">
+      <c r="G10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="79"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="70"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="2"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="70"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="70"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="70"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="70"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="70"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="70"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="68"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="4"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1218,12 +1223,12 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="74"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -1231,80 +1236,80 @@
       <c r="K24" s="13"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="71" t="s">
+      <c r="C25" s="36"/>
+      <c r="D25" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71" t="s">
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71" t="s">
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="72"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="44" t="s">
+      <c r="C27" s="38"/>
+      <c r="D27" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="31" t="s">
+      <c r="E27" s="79"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="87" t="s">
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="57"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="52"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
@@ -1349,16 +1354,16 @@
       <c r="L31" s="20"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="4"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1366,7 +1371,7 @@
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="76"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
@@ -1379,116 +1384,116 @@
       <c r="K33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="37" t="s">
+      <c r="C34" s="61"/>
+      <c r="D34" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37" t="s">
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37" t="s">
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>1</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28" t="s">
+      <c r="C36" s="31"/>
+      <c r="D36" s="70" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="39" t="s">
+      <c r="F36" s="71"/>
+      <c r="G36" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="55" t="s">
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="57"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="52"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
+      <c r="A40" s="59"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
       <c r="G40" s="4"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -1496,12 +1501,12 @@
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
+      <c r="A41" s="59"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
@@ -1509,54 +1514,54 @@
       <c r="K41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="77"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="61"/>
+      <c r="L42" s="61"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="28"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="29"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="75"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
+      <c r="A47" s="59"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1564,12 +1569,12 @@
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="49"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
@@ -1577,54 +1582,54 @@
       <c r="K48" s="13"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="28"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="70"/>
       <c r="E51" s="29"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="42"/>
-      <c r="L51" s="43"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="85"/>
+      <c r="K51" s="86"/>
+      <c r="L51" s="87"/>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
+      <c r="A55" s="59"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
       <c r="G55" s="4"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -1632,12 +1637,12 @@
       <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="36"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
+      <c r="A56" s="59"/>
+      <c r="B56" s="74"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
@@ -1645,68 +1650,68 @@
       <c r="K56" s="13"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="38"/>
-      <c r="L57" s="38"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="60"/>
+      <c r="J57" s="60"/>
+      <c r="K57" s="61"/>
+      <c r="L57" s="61"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="38"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="38"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="61"/>
+      <c r="K58" s="61"/>
+      <c r="L58" s="61"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="28"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="29"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="34"/>
-      <c r="L59" s="35"/>
+      <c r="F59" s="71"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="75"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="83"/>
+      <c r="L59" s="84"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="28"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="70"/>
       <c r="E60" s="29"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="35"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="74"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="75"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="83"/>
+      <c r="L60" s="84"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="36"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
+      <c r="A63" s="59"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
       <c r="G63" s="4"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -1714,12 +1719,12 @@
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="36"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
+      <c r="A64" s="59"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
+      <c r="F64" s="74"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
@@ -1727,46 +1732,46 @@
       <c r="K64" s="13"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
+      <c r="A65" s="60"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="60"/>
+      <c r="J65" s="60"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="61"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="38"/>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
-      <c r="I66" s="37"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
+      <c r="A66" s="61"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="60"/>
+      <c r="J66" s="61"/>
+      <c r="K66" s="61"/>
+      <c r="L66" s="61"/>
     </row>
     <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="28"/>
+      <c r="B67" s="66"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="70"/>
       <c r="E67" s="29"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="34"/>
-      <c r="L67" s="35"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="75"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="82"/>
+      <c r="K67" s="83"/>
+      <c r="L67" s="84"/>
     </row>
     <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="22"/>
@@ -3103,6 +3108,96 @@
     </row>
   </sheetData>
   <mergeCells count="114">
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="J60:L60"/>
+    <mergeCell ref="B55:F56"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G49:I50"/>
+    <mergeCell ref="J49:L50"/>
+    <mergeCell ref="B47:F48"/>
+    <mergeCell ref="B40:F41"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G65:I66"/>
+    <mergeCell ref="J65:L66"/>
+    <mergeCell ref="B63:F64"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="D65:F66"/>
+    <mergeCell ref="J57:L58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="J59:L59"/>
+    <mergeCell ref="B57:C58"/>
+    <mergeCell ref="D57:F58"/>
+    <mergeCell ref="G57:I58"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="D42:F43"/>
+    <mergeCell ref="G42:I43"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:F50"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:F35"/>
+    <mergeCell ref="G34:I35"/>
+    <mergeCell ref="J42:L43"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J34:L35"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="J25:L26"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G25:I26"/>
+    <mergeCell ref="D25:F26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B23:F24"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:F33"/>
     <mergeCell ref="B11:D11"/>
@@ -3127,96 +3222,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="J28:L28"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="J25:L26"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G25:I26"/>
-    <mergeCell ref="D25:F26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B23:F24"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:F35"/>
-    <mergeCell ref="G34:I35"/>
-    <mergeCell ref="J42:L43"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J34:L35"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="D42:F43"/>
-    <mergeCell ref="G42:I43"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:F50"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G49:I50"/>
-    <mergeCell ref="J49:L50"/>
-    <mergeCell ref="B47:F48"/>
-    <mergeCell ref="B40:F41"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G65:I66"/>
-    <mergeCell ref="J65:L66"/>
-    <mergeCell ref="B63:F64"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="D65:F66"/>
-    <mergeCell ref="J57:L58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="J59:L59"/>
-    <mergeCell ref="B57:C58"/>
-    <mergeCell ref="D57:F58"/>
-    <mergeCell ref="G57:I58"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="J60:L60"/>
-    <mergeCell ref="B55:F56"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>